<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@b2e51206528f1b6ae8ac0e6dcaabf5c8ee8544cf 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.2.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="166">
   <si>
     <t>Row</t>
   </si>
@@ -212,7 +212,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>J101 J102 J103 J104</t>
+    <t>J101 J102 J103 J104 J105</t>
   </si>
   <si>
     <t>Conn_01x02</t>
@@ -275,7 +275,22 @@
     <t>11</t>
   </si>
   <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117 R118</t>
+    <t>Q101</t>
+  </si>
+  <si>
+    <t>AO3400A</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>30V Vds, 5.7A Id, N-Channel MOSFET, SOT-23</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117 R118 R119 R120 R121</t>
   </si>
   <si>
     <t>R</t>
@@ -296,105 +311,105 @@
     <t>Resistor</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>SW101 SW102</t>
+  </si>
+  <si>
+    <t>SW_Push_45deg</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/tact-64n-f/microswitches-tact/ninigi/</t>
+  </si>
+  <si>
+    <t>SW_PUSH_6mm</t>
+  </si>
+  <si>
+    <t>Push button switch, normally open, two pins, 45° tilted</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>AT24CS64-SSHM</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-T</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/MicrochipTech-AT24C256C_SSHLT/C6482</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>U104</t>
+  </si>
+  <si>
+    <t>ATECC608A-MAHDA</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/MicrochipTech-ATECC608B_MAHDAT/C17561150</t>
+  </si>
+  <si>
+    <t>DFN-8-1EP_3x2mm_P0.5mm_EP1.3x1.5mm</t>
+  </si>
+  <si>
+    <t>Cryptographic Co-Processor with Secure Hardware-based 16 Key Storage, ECDSA and ECDH support, I2C, UDFN-8</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>U105</t>
+  </si>
+  <si>
+    <t>DS3231MZ</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/108629-DS3231MZTRL/C107410</t>
+  </si>
+  <si>
+    <t>±5ppm, I2C Real-Time Clock SOIC-8</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>U202</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/3522416-ESP32_S3_WROOM_1UN16R8/C3013946</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1U</t>
+  </si>
+  <si>
+    <t>2.4 GHz WiFi (802.11 b/g/n) and Bluetooth ® 5 (LE) module Built around ESP32S3 series of SoCs, Xtensa ® dualcore 32bit LX7 microprocessor Flash up to 16 MB, PSRAM up to 8 MB 36 GPIOs, rich set of peripherals Onboard PCB antenna</t>
+  </si>
+  <si>
     <t>18</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>SW101 SW102</t>
-  </si>
-  <si>
-    <t>SW_Push_45deg</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/tact-64n-f/microswitches-tact/ninigi/</t>
-  </si>
-  <si>
-    <t>SW_PUSH_6mm</t>
-  </si>
-  <si>
-    <t>Push button switch, normally open, two pins, 45° tilted</t>
-  </si>
-  <si>
-    <t>U103</t>
-  </si>
-  <si>
-    <t>AT24CS64-SSHM</t>
-  </si>
-  <si>
-    <t>AT24C512C-SSHD-T</t>
-  </si>
-  <si>
-    <t>Microchip Tech</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/MicrochipTech-AT24C256C_SSHLT/C6482</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>U104</t>
-  </si>
-  <si>
-    <t>ATECC608A-MAHDA</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/MicrochipTech-ATECC608B_MAHDAT/C17561150</t>
-  </si>
-  <si>
-    <t>DFN-8-1EP_3x2mm_P0.5mm_EP1.3x1.5mm</t>
-  </si>
-  <si>
-    <t>Cryptographic Co-Processor with Secure Hardware-based 16 Key Storage, ECDSA and ECDH support, I2C, UDFN-8</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>U105</t>
-  </si>
-  <si>
-    <t>DS3231MZ</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/108629-DS3231MZTRL/C107410</t>
-  </si>
-  <si>
-    <t>±5ppm, I2C Real-Time Clock SOIC-8</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>U202</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-1</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/3522416-ESP32_S3_WROOM_1UN16R8/C3013946</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-1U</t>
-  </si>
-  <si>
-    <t>2.4 GHz WiFi (802.11 b/g/n) and Bluetooth ® 5 (LE) module Built around ESP32S3 series of SoCs, Xtensa ® dualcore 32bit LX7 microprocessor Flash up to 16 MB, PSRAM up to 8 MB 36 GPIOs, rich set of peripherals Onboard PCB antenna</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>U102</t>
   </si>
   <si>
@@ -407,6 +422,9 @@
     <t>https://www.tme.eu/de/en/details/r-78k5.0-0.5/dc-dc-converters/recom/</t>
   </si>
   <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>U101</t>
   </si>
   <si>
@@ -422,7 +440,7 @@
     <t>Industrial 3.3V Low Power Half-Duplex RS-485 Transceiver 10Mbps, SOIC-8</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>U201</t>
@@ -976,7 +994,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1001,7 +1019,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1015,55 +1033,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="F2" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F3" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F4" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1071,16 +1089,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F6" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1422,7 +1440,7 @@
         <v>70</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
@@ -1501,7 +1519,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="30" customHeight="1">
+    <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
         <v>84</v>
       </c>
@@ -1512,69 +1530,69 @@
         <v>86</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="L19" s="5" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="G20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="J20" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="K20" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="10" t="s">
+      <c r="L20" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
@@ -1582,57 +1600,57 @@
         <v>43</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="K21" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="L21" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="E22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>18</v>
@@ -1641,30 +1659,30 @@
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="K22" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>115</v>
-      </c>
       <c r="D23" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1679,10 +1697,10 @@
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>117</v>
@@ -1691,7 +1709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="60" customHeight="1">
+    <row r="24" spans="1:12">
       <c r="A24" s="8" t="s">
         <v>118</v>
       </c>
@@ -1720,48 +1738,48 @@
         <v>121</v>
       </c>
       <c r="J24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="K24" s="10" t="s">
-        <v>123</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1">
+    <row r="25" spans="1:12" ht="60" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="J25" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="7" t="s">
+      <c r="K25" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>12</v>
@@ -1769,37 +1787,37 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="K26" s="10" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>12</v>
@@ -1822,7 +1840,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>18</v>
@@ -1831,15 +1849,53 @@
         <v>16</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>139</v>
       </c>
       <c r="L27" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="L28" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1867,10 +1923,11 @@
     <hyperlink ref="H25" r:id="rId17"/>
     <hyperlink ref="H26" r:id="rId18"/>
     <hyperlink ref="H27" r:id="rId19"/>
+    <hyperlink ref="H28" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId20"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -1887,22 +1944,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@ad5f9b1a2a3626d344ceb5e74cdc26189343dac5 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.2.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.2.xlsx
@@ -176,13 +176,13 @@
     <t>D201</t>
   </si>
   <si>
-    <t>SK6812MINI</t>
+    <t>SK6812MINI-HS-012</t>
   </si>
   <si>
     <t>https://jlcpcb.com/partdetail/OPSCOOptoelectronics-SK6812MINIHS/C2922787</t>
   </si>
   <si>
-    <t>LED_SK6812MINI_PLCC4_3.5x3.5mm_P1.75mm</t>
+    <t>LED_WS2812B-Mini_PLCC4_3.5x3.5mm</t>
   </si>
   <si>
     <t>RGB LED with integrated controller</t>

</xml_diff>